<commit_message>
fix: schema mapping (#17)
* feat: id4africa demo

Signed-off-by: Sai Ranjit Tummalapalli <sairanjit.tummalapalli@ayanworks.com>

* resolve conflicts

Signed-off-by: Sai Ranjit Tummalapalli <sairanjit.tummalapalli@ayanworks.com>

* fix: schema

Signed-off-by: Sai Ranjit Tummalapalli <sairanjit.tummalapalli@ayanworks.com>

---------

Signed-off-by: Sai Ranjit Tummalapalli <sairanjit.tummalapalli@ayanworks.com>
</commit_message>
<xml_diff>
--- a/OCABundles/schema/credebl/id4africa-delegate/Delegate.xlsx
+++ b/OCABundles/schema/credebl/id4africa-delegate/Delegate.xlsx
@@ -1171,7 +1171,7 @@
     <t>name</t>
   </si>
   <si>
-    <t>Speaker</t>
+    <t>Delegate</t>
   </si>
   <si>
     <t>Full Name</t>
@@ -1180,7 +1180,7 @@
     <t>description</t>
   </si>
   <si>
-    <t>Speaker Schema</t>
+    <t>Delegate Schema</t>
   </si>
   <si>
     <t>Phone</t>
@@ -2219,7 +2219,7 @@
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="50" fillId="9" fontId="17" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="51" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
@@ -2234,7 +2234,7 @@
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="33" fillId="9" fontId="17" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="55" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>

</xml_diff>